<commit_message>
Restore from tablet 2
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emil\Code\ODKX\celsos\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\celso\odkx\QPS2020\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C1DC46-BCDB-4ACB-A1A0-48D18A2A91A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B05113-5447-40BD-8F6D-FBC1B223E5CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -19,14 +19,8 @@
     <sheet name="choices" sheetId="6" r:id="rId4"/>
     <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="229">
   <si>
     <t>comments</t>
   </si>
@@ -508,6 +502,18 @@
     <t>en</t>
   </si>
   <si>
+    <t>QPS</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('QPS')</t>
+  </si>
+  <si>
+    <t>inscricao</t>
+  </si>
+  <si>
+    <t>Quimioprevenção do Paludismo Sazonal</t>
+  </si>
+  <si>
     <t>Escolha o formulário</t>
   </si>
   <si>
@@ -721,64 +727,19 @@
     <t>Você tem certeza que quere sair e perder todas as alterações?</t>
   </si>
   <si>
-    <t>inclusao</t>
-  </si>
-  <si>
-    <t>laboratorio</t>
-  </si>
-  <si>
-    <t>rastreio</t>
-  </si>
-  <si>
-    <t>seguimento</t>
-  </si>
-  <si>
-    <t>Formulário de inclusão de caso: Dia 0</t>
-  </si>
-  <si>
-    <t>Formulário de reportagem de evento adverso</t>
-  </si>
-  <si>
-    <t>evento_adverso</t>
-  </si>
-  <si>
-    <t>Resultados de laboratorio</t>
-  </si>
-  <si>
-    <t>Rastreio de caso</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('laboratorio')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('evento_adverso')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('rastreio')</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('seguimento')</t>
-  </si>
-  <si>
-    <t>Seguimento</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('inclusao')</t>
-  </si>
-  <si>
-    <t>outroDia</t>
-  </si>
-  <si>
-    <t>Seguimento de qualquer outro Dia</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('outroDia')</t>
-  </si>
-  <si>
-    <t>codigos</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('codigos')</t>
+    <t xml:space="preserve">Inscricao </t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('QPS','inscricao')</t>
+  </si>
+  <si>
+    <t>ronda</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('ronda')</t>
+  </si>
+  <si>
+    <t>Rondas</t>
   </si>
 </sst>
 </file>
@@ -1357,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1392,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1453,7 +1414,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1483,180 +1444,95 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" t="s">
         <v>28</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" t="s">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="E14" t="s">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17" t="s">
         <v>28</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" t="s">
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E33" t="s">
-        <v>28</v>
-      </c>
-      <c r="G33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" t="s">
-        <v>27</v>
-      </c>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1673,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1694,13 +1570,13 @@
         <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
         <v>151</v>
       </c>
       <c r="F1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -1741,7 +1617,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>2020071900</v>
+        <v>2019082600</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
@@ -1755,7 +1631,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -1772,18 +1648,18 @@
         <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1868,17 +1744,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="63.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1897,10 +1773,10 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>222</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1908,65 +1784,21 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>224</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>223</v>
-      </c>
-      <c r="C4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B4" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>236</v>
+      <c r="C4" s="9" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +1817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
@@ -2004,7 +1836,7 @@
         <v>54</v>
       </c>
       <c r="C1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2015,7 +1847,7 @@
         <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2026,7 +1858,7 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2037,7 +1869,7 @@
         <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2048,7 +1880,7 @@
         <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2059,7 +1891,7 @@
         <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2070,7 +1902,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2081,7 +1913,7 @@
         <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2092,7 +1924,7 @@
         <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2103,7 +1935,7 @@
         <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -2114,7 +1946,7 @@
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -2125,7 +1957,7 @@
         <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2136,7 +1968,7 @@
         <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2180,7 +2012,7 @@
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2191,7 +2023,7 @@
         <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2202,7 +2034,7 @@
         <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2213,7 +2045,7 @@
         <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -2224,7 +2056,7 @@
         <v>74</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2235,7 +2067,7 @@
         <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2246,7 +2078,7 @@
         <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2257,7 +2089,7 @@
         <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2268,7 +2100,7 @@
         <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2279,7 +2111,7 @@
         <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2290,7 +2122,7 @@
         <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2301,7 +2133,7 @@
         <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
@@ -2312,7 +2144,7 @@
         <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2323,7 +2155,7 @@
         <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2334,7 +2166,7 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2345,7 +2177,7 @@
         <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2356,7 +2188,7 @@
         <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2367,7 +2199,7 @@
         <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="165.75" x14ac:dyDescent="0.2">
@@ -2378,7 +2210,7 @@
         <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2389,7 +2221,7 @@
         <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2400,7 +2232,7 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2411,7 +2243,7 @@
         <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2422,7 +2254,7 @@
         <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2433,7 +2265,7 @@
         <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2444,7 +2276,7 @@
         <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2455,7 +2287,7 @@
         <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2466,7 +2298,7 @@
         <v>122</v>
       </c>
       <c r="C44" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2477,7 +2309,7 @@
         <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2488,7 +2320,7 @@
         <v>141</v>
       </c>
       <c r="C46" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -2499,7 +2331,7 @@
         <v>127</v>
       </c>
       <c r="C47" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -2510,7 +2342,7 @@
         <v>129</v>
       </c>
       <c r="C48" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
@@ -2521,7 +2353,7 @@
         <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2532,7 +2364,7 @@
         <v>133</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
@@ -2543,7 +2375,7 @@
         <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -2554,7 +2386,7 @@
         <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
@@ -2565,7 +2397,7 @@
         <v>135</v>
       </c>
       <c r="C53" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
@@ -2576,7 +2408,7 @@
         <v>127</v>
       </c>
       <c r="C54" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
@@ -2587,7 +2419,7 @@
         <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -2598,7 +2430,7 @@
         <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2609,40 +2441,40 @@
         <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C59" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C60" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>